<commit_message>
Add VS680 test Script and test case
</commit_message>
<xml_diff>
--- a/VS680_Scripts/vs680scripts/launchTimeTest/APP启动时间.xlsx
+++ b/VS680_Scripts/vs680scripts/launchTimeTest/APP启动时间.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\VS680_Scripts\vs680scripts\launchTimeTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\pythonProject_seevision\VS680_Scripts\vs680scripts\launchTimeTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0FD436-CA61-419B-A7CF-1E959F29BB30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE74EC79-07DD-4E3B-B9A7-738672C9C7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="result" sheetId="1" r:id="rId1"/>
@@ -1504,20 +1504,20 @@
   <dimension ref="A1:B531"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="16.7265625" customWidth="1"/>
+    <col min="1" max="2" width="16.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -3237,7 +3237,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -3333,7 +3333,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -3445,7 +3445,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -3533,7 +3533,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A260" s="1">
         <v>258</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -3613,7 +3613,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A265" s="1">
         <v>263</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A267" s="1">
         <v>265</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A269" s="1">
         <v>267</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A274" s="1">
         <v>272</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A275" s="1">
         <v>273</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A276" s="1">
         <v>274</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A277" s="1">
         <v>275</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A278" s="1">
         <v>276</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A279" s="1">
         <v>277</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A280" s="1">
         <v>278</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A281" s="1">
         <v>279</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A282" s="1">
         <v>280</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A283" s="1">
         <v>281</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A284" s="1">
         <v>282</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A285" s="1">
         <v>283</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A286" s="1">
         <v>284</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A287" s="1">
         <v>285</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A288" s="1">
         <v>286</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A289" s="1">
         <v>287</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A290" s="1">
         <v>288</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A291" s="1">
         <v>289</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A292" s="1">
         <v>290</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A293" s="1">
         <v>291</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A294" s="1">
         <v>292</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A295" s="1">
         <v>293</v>
       </c>
@@ -3869,7 +3869,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A296" s="1">
         <v>294</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A297" s="1">
         <v>295</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A298" s="1">
         <v>296</v>
       </c>
@@ -3893,7 +3893,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A299" s="1">
         <v>297</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A300" s="1">
         <v>298</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A301" s="1">
         <v>299</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A302" s="1">
         <v>300</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A303" s="1">
         <v>301</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A304" s="1">
         <v>302</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A305" s="1">
         <v>303</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A306" s="1">
         <v>304</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A307" s="1">
         <v>305</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A308" s="1">
         <v>306</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A309" s="1">
         <v>307</v>
       </c>
@@ -3981,7 +3981,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A310" s="1">
         <v>308</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A311" s="1">
         <v>309</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A312" s="1">
         <v>310</v>
       </c>
@@ -4005,7 +4005,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A313" s="1">
         <v>311</v>
       </c>
@@ -4013,7 +4013,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A314" s="1">
         <v>312</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A315" s="1">
         <v>313</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A316" s="1">
         <v>314</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A317" s="1">
         <v>315</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A318" s="1">
         <v>316</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A319" s="1">
         <v>317</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A320" s="1">
         <v>318</v>
       </c>
@@ -4069,7 +4069,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A321" s="1">
         <v>319</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A322" s="1">
         <v>320</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A323" s="1">
         <v>321</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A324" s="1">
         <v>322</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A325" s="1">
         <v>323</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A326" s="1">
         <v>324</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A327" s="1">
         <v>325</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A328" s="1">
         <v>326</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A329" s="1">
         <v>327</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A330" s="1">
         <v>328</v>
       </c>
@@ -4149,7 +4149,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A331" s="1">
         <v>329</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A332" s="1">
         <v>330</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A333" s="1">
         <v>331</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A334" s="1">
         <v>332</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A335" s="1">
         <v>333</v>
       </c>
@@ -4189,7 +4189,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A336" s="1">
         <v>334</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A337" s="1">
         <v>335</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A338" s="1">
         <v>336</v>
       </c>
@@ -4213,7 +4213,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A339" s="1">
         <v>337</v>
       </c>
@@ -4221,7 +4221,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A340" s="1">
         <v>338</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A341" s="1">
         <v>339</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A342" s="1">
         <v>340</v>
       </c>
@@ -4245,7 +4245,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A343" s="1">
         <v>341</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A344" s="1">
         <v>342</v>
       </c>
@@ -4261,7 +4261,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A345" s="1">
         <v>343</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A346" s="1">
         <v>344</v>
       </c>
@@ -4277,7 +4277,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A347" s="1">
         <v>345</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A348" s="1">
         <v>346</v>
       </c>
@@ -4293,7 +4293,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A349" s="1">
         <v>347</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A350" s="1">
         <v>348</v>
       </c>
@@ -4309,7 +4309,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A351" s="1">
         <v>349</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A352" s="1">
         <v>350</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A353" s="1">
         <v>351</v>
       </c>
@@ -4333,7 +4333,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A354" s="1">
         <v>352</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A355" s="1">
         <v>353</v>
       </c>
@@ -4349,7 +4349,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A356" s="1">
         <v>354</v>
       </c>
@@ -4357,7 +4357,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A357" s="1">
         <v>355</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A358" s="1">
         <v>356</v>
       </c>
@@ -4373,7 +4373,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A359" s="1">
         <v>357</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A360" s="1">
         <v>358</v>
       </c>
@@ -4389,7 +4389,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A361" s="1">
         <v>359</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A362" s="1">
         <v>360</v>
       </c>
@@ -4405,7 +4405,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A363" s="1">
         <v>361</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A364" s="1">
         <v>362</v>
       </c>
@@ -4421,7 +4421,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A365" s="1">
         <v>363</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A366" s="1">
         <v>364</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A367" s="1">
         <v>365</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A368" s="1">
         <v>366</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A369" s="1">
         <v>367</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A370" s="1">
         <v>368</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A371" s="1">
         <v>369</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A372" s="1">
         <v>370</v>
       </c>
@@ -4485,7 +4485,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A373" s="1">
         <v>371</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A374" s="1">
         <v>372</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A375" s="1">
         <v>373</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A376" s="1">
         <v>374</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A377" s="1">
         <v>375</v>
       </c>
@@ -4525,7 +4525,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A378" s="1">
         <v>376</v>
       </c>
@@ -4533,7 +4533,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A379" s="1">
         <v>377</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A380" s="1">
         <v>378</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A381" s="1">
         <v>379</v>
       </c>
@@ -4557,7 +4557,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A382" s="1">
         <v>380</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A383" s="1">
         <v>381</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A384" s="1">
         <v>382</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A385" s="1">
         <v>383</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A386" s="1">
         <v>384</v>
       </c>
@@ -4597,7 +4597,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A387" s="1">
         <v>385</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A388" s="1">
         <v>386</v>
       </c>
@@ -4613,7 +4613,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A389" s="1">
         <v>387</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A390" s="1">
         <v>388</v>
       </c>
@@ -4629,7 +4629,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A391" s="1">
         <v>389</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A392" s="1">
         <v>390</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A393" s="1">
         <v>391</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A394" s="1">
         <v>392</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A395" s="1">
         <v>393</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A396" s="1">
         <v>394</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A397" s="1">
         <v>395</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A398" s="1">
         <v>396</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A399" s="1">
         <v>397</v>
       </c>
@@ -4701,7 +4701,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A400" s="1">
         <v>398</v>
       </c>
@@ -4709,7 +4709,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A401" s="1">
         <v>399</v>
       </c>
@@ -4717,7 +4717,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A402" s="1">
         <v>400</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A403" s="1">
         <v>401</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A404" s="1">
         <v>402</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A405" s="1">
         <v>403</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A406" s="1">
         <v>404</v>
       </c>
@@ -4757,7 +4757,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A407" s="1">
         <v>405</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A408" s="1">
         <v>406</v>
       </c>
@@ -4773,7 +4773,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A409" s="1">
         <v>407</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A410" s="1">
         <v>408</v>
       </c>
@@ -4789,7 +4789,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A411" s="1">
         <v>409</v>
       </c>
@@ -4797,7 +4797,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A412" s="1">
         <v>410</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A413" s="1">
         <v>411</v>
       </c>
@@ -4813,7 +4813,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A414" s="1">
         <v>412</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A415" s="1">
         <v>413</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A416" s="1">
         <v>414</v>
       </c>
@@ -4837,7 +4837,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A417" s="1">
         <v>415</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A418" s="1">
         <v>416</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A419" s="1">
         <v>417</v>
       </c>
@@ -4861,7 +4861,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A420" s="1">
         <v>418</v>
       </c>
@@ -4869,7 +4869,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A421" s="1">
         <v>419</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A422" s="1">
         <v>420</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A423" s="1">
         <v>421</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A424" s="1">
         <v>422</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A425" s="1">
         <v>423</v>
       </c>
@@ -4909,7 +4909,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A426" s="1">
         <v>424</v>
       </c>
@@ -4917,7 +4917,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A427" s="1">
         <v>425</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A428" s="1">
         <v>426</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A429" s="1">
         <v>427</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A430" s="1">
         <v>428</v>
       </c>
@@ -4949,7 +4949,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A431" s="1">
         <v>429</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A432" s="1">
         <v>430</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A433" s="1">
         <v>431</v>
       </c>
@@ -4973,7 +4973,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A434" s="1">
         <v>432</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A435" s="1">
         <v>433</v>
       </c>
@@ -4989,7 +4989,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A436" s="1">
         <v>434</v>
       </c>
@@ -4997,7 +4997,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A437" s="1">
         <v>435</v>
       </c>
@@ -5005,7 +5005,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A438" s="1">
         <v>436</v>
       </c>
@@ -5013,7 +5013,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A439" s="1">
         <v>437</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A440" s="1">
         <v>438</v>
       </c>
@@ -5029,7 +5029,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A441" s="1">
         <v>439</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A442" s="1">
         <v>440</v>
       </c>
@@ -5045,7 +5045,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A443" s="1">
         <v>441</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A444" s="1">
         <v>442</v>
       </c>
@@ -5061,7 +5061,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A445" s="1">
         <v>443</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A446" s="1">
         <v>444</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A447" s="1">
         <v>445</v>
       </c>
@@ -5085,7 +5085,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A448" s="1">
         <v>446</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A449" s="1">
         <v>447</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="450" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A450" s="1">
         <v>448</v>
       </c>
@@ -5109,7 +5109,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A451" s="1">
         <v>449</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="452" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A452" s="1">
         <v>450</v>
       </c>
@@ -5125,7 +5125,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="453" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A453" s="1">
         <v>451</v>
       </c>
@@ -5133,7 +5133,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="454" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A454" s="1">
         <v>452</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A455" s="1">
         <v>453</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A456" s="1">
         <v>454</v>
       </c>
@@ -5157,7 +5157,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="457" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A457" s="1">
         <v>455</v>
       </c>
@@ -5165,7 +5165,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="458" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A458" s="1">
         <v>456</v>
       </c>
@@ -5173,7 +5173,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A459" s="1">
         <v>457</v>
       </c>
@@ -5181,7 +5181,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A460" s="1">
         <v>458</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="461" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A461" s="1">
         <v>459</v>
       </c>
@@ -5197,7 +5197,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="462" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A462" s="1">
         <v>460</v>
       </c>
@@ -5205,7 +5205,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="463" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A463" s="1">
         <v>461</v>
       </c>
@@ -5213,7 +5213,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="464" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A464" s="1">
         <v>462</v>
       </c>
@@ -5221,7 +5221,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="465" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A465" s="1">
         <v>463</v>
       </c>
@@ -5229,7 +5229,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="466" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A466" s="1">
         <v>464</v>
       </c>
@@ -5237,7 +5237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A467" s="1">
         <v>465</v>
       </c>
@@ -5245,7 +5245,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A468" s="1">
         <v>466</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A469" s="1">
         <v>467</v>
       </c>
@@ -5261,7 +5261,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A470" s="1">
         <v>468</v>
       </c>
@@ -5269,7 +5269,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A471" s="1">
         <v>469</v>
       </c>
@@ -5277,7 +5277,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A472" s="1">
         <v>470</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A473" s="1">
         <v>471</v>
       </c>
@@ -5293,7 +5293,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="474" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A474" s="1">
         <v>472</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A475" s="1">
         <v>473</v>
       </c>
@@ -5309,7 +5309,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="476" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A476" s="1">
         <v>474</v>
       </c>
@@ -5317,7 +5317,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="477" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A477" s="1">
         <v>475</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="478" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A478" s="1">
         <v>476</v>
       </c>
@@ -5333,7 +5333,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="479" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A479" s="1">
         <v>477</v>
       </c>
@@ -5341,7 +5341,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="480" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A480" s="1">
         <v>478</v>
       </c>
@@ -5349,7 +5349,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="481" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A481" s="1">
         <v>479</v>
       </c>
@@ -5357,7 +5357,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="482" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A482" s="1">
         <v>480</v>
       </c>
@@ -5365,7 +5365,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="483" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A483" s="1">
         <v>481</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="484" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A484" s="1">
         <v>482</v>
       </c>
@@ -5381,7 +5381,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="485" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A485" s="1">
         <v>483</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="486" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A486" s="1">
         <v>484</v>
       </c>
@@ -5397,7 +5397,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="487" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A487" s="1">
         <v>485</v>
       </c>
@@ -5405,7 +5405,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="488" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A488" s="1">
         <v>486</v>
       </c>
@@ -5413,7 +5413,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="489" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A489" s="1">
         <v>487</v>
       </c>
@@ -5421,7 +5421,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="490" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A490" s="1">
         <v>488</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="491" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A491" s="1">
         <v>489</v>
       </c>
@@ -5437,7 +5437,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="492" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A492" s="1">
         <v>490</v>
       </c>
@@ -5445,7 +5445,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="493" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A493" s="1">
         <v>491</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="494" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A494" s="1">
         <v>492</v>
       </c>
@@ -5461,7 +5461,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="495" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A495" s="1">
         <v>493</v>
       </c>
@@ -5469,7 +5469,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="496" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A496" s="1">
         <v>494</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="497" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A497" s="1">
         <v>495</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="498" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A498" s="1">
         <v>496</v>
       </c>
@@ -5493,7 +5493,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="499" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A499" s="1">
         <v>497</v>
       </c>
@@ -5501,7 +5501,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="500" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A500" s="1">
         <v>498</v>
       </c>
@@ -5509,7 +5509,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="501" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A501" s="1">
         <v>499</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="502" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A502" s="1">
         <v>500</v>
       </c>
@@ -5525,7 +5525,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="503" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A503" s="1">
         <v>501</v>
       </c>
@@ -5533,7 +5533,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="504" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A504" s="1">
         <v>502</v>
       </c>
@@ -5541,7 +5541,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="505" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A505" s="1">
         <v>503</v>
       </c>
@@ -5549,7 +5549,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="506" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A506" s="1">
         <v>504</v>
       </c>
@@ -5557,7 +5557,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="507" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A507" s="1">
         <v>505</v>
       </c>
@@ -5565,7 +5565,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="508" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A508" s="1">
         <v>506</v>
       </c>
@@ -5573,7 +5573,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="509" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A509" s="1">
         <v>507</v>
       </c>
@@ -5581,7 +5581,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="510" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A510" s="1">
         <v>508</v>
       </c>
@@ -5589,7 +5589,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="511" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A511" s="1">
         <v>509</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="512" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A512" s="1">
         <v>510</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="513" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A513" s="1">
         <v>511</v>
       </c>
@@ -5613,7 +5613,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="514" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A514" s="1">
         <v>512</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="515" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A515" s="1">
         <v>513</v>
       </c>
@@ -5629,7 +5629,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="516" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A516" s="1">
         <v>514</v>
       </c>
@@ -5637,7 +5637,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="517" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A517" s="1">
         <v>515</v>
       </c>
@@ -5645,7 +5645,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="518" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A518" s="1">
         <v>516</v>
       </c>
@@ -5653,7 +5653,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="519" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A519" s="1">
         <v>517</v>
       </c>
@@ -5661,7 +5661,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="520" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A520" s="1">
         <v>518</v>
       </c>
@@ -5669,7 +5669,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="521" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A521" s="1">
         <v>519</v>
       </c>
@@ -5677,7 +5677,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="522" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A522" s="1">
         <v>520</v>
       </c>
@@ -5685,7 +5685,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="523" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A523" s="1">
         <v>521</v>
       </c>
@@ -5693,7 +5693,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="524" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A524" s="1">
         <v>522</v>
       </c>
@@ -5701,7 +5701,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="525" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A525" s="1">
         <v>523</v>
       </c>
@@ -5709,7 +5709,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="526" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A526" s="1">
         <v>524</v>
       </c>
@@ -5717,7 +5717,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="527" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A527" s="1">
         <v>525</v>
       </c>
@@ -5725,7 +5725,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="528" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A528" s="1">
         <v>526</v>
       </c>
@@ -5733,7 +5733,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="529" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A529" s="1">
         <v>527</v>
       </c>
@@ -5741,7 +5741,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="530" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A530" s="1">
         <v>528</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="531" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A531" s="1">
         <v>529</v>
       </c>

</xml_diff>